<commit_message>
Fixed error in input data, changed data structure of time series
</commit_message>
<xml_diff>
--- a/input_data/input_data_V3.xlsx
+++ b/input_data/input_data_V3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dsdennis\HOPE\Predicer\input_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0BDB3AF-7277-4FC1-AD5C-920A3C1FB5F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B96AC75-ECF7-40C9-AD56-759F416A340C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="796" activeTab="6" xr2:uid="{788BFBD1-D930-4535-8A91-D85C56924796}"/>
+    <workbookView xWindow="30" yWindow="0" windowWidth="20460" windowHeight="10920" tabRatio="796" activeTab="2" xr2:uid="{788BFBD1-D930-4535-8A91-D85C56924796}"/>
   </bookViews>
   <sheets>
     <sheet name="nodes" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="73">
   <si>
     <t>node</t>
   </si>
@@ -136,9 +136,6 @@
   </si>
   <si>
     <t>VOM_cost</t>
-  </si>
-  <si>
-    <t>p2x</t>
   </si>
   <si>
     <t>t</t>
@@ -638,7 +635,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E1" t="s">
         <v>6</v>
@@ -774,7 +771,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -859,7 +856,7 @@
         <v>15</v>
       </c>
       <c r="D1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E1" t="s">
         <v>18</v>
@@ -1010,7 +1007,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -1081,8 +1078,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A86A8A7-FD76-4891-A53C-CBB095359118}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1103,7 +1100,7 @@
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E1" t="s">
         <v>16</v>
@@ -1214,7 +1211,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="B7" t="s">
         <v>28</v>
@@ -1234,7 +1231,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="B8" t="s">
         <v>30</v>
@@ -1274,7 +1271,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B10" t="s">
         <v>28</v>
@@ -1294,13 +1291,13 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B11" t="s">
         <v>30</v>
       </c>
       <c r="C11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -1369,7 +1366,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B1" t="s">
         <v>26</v>
@@ -1377,7 +1374,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -1385,7 +1382,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B3">
         <v>0.4</v>
@@ -1393,7 +1390,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B4">
         <v>0.5</v>
@@ -1401,7 +1398,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -1409,7 +1406,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B6">
         <v>0.8</v>
@@ -1417,7 +1414,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -1425,7 +1422,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B8">
         <v>0.1</v>
@@ -1433,7 +1430,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B9">
         <v>0.6</v>
@@ -1441,7 +1438,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B10">
         <v>0.4</v>
@@ -1449,7 +1446,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B11">
         <v>0.6</v>
@@ -1457,7 +1454,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B12">
         <v>0.7</v>
@@ -1465,7 +1462,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B13">
         <v>0.1</v>
@@ -1473,7 +1470,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B14">
         <v>0.1</v>
@@ -1481,7 +1478,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B15">
         <v>0.8</v>
@@ -1489,7 +1486,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B16">
         <v>0.9</v>
@@ -1497,7 +1494,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B17">
         <v>0.2</v>
@@ -1505,7 +1502,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B18">
         <v>0.4</v>
@@ -1513,7 +1510,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B19">
         <v>0.6</v>
@@ -1521,7 +1518,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B20">
         <v>0.7</v>
@@ -1529,7 +1526,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B21">
         <v>0.7</v>
@@ -1537,7 +1534,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B22">
         <v>0.6</v>
@@ -1545,7 +1542,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B23">
         <v>0.7</v>
@@ -1553,7 +1550,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B24">
         <v>0.1</v>
@@ -1561,7 +1558,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B25">
         <v>0.6</v>
@@ -1585,10 +1582,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C1" t="s">
         <v>11</v>
@@ -1596,7 +1593,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B2">
         <v>12</v>
@@ -1607,7 +1604,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B3">
         <v>15</v>
@@ -1618,7 +1615,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -1629,7 +1626,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B5">
         <v>15</v>
@@ -1640,7 +1637,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B6">
         <v>3</v>
@@ -1651,7 +1648,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B7">
         <v>9</v>
@@ -1662,7 +1659,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B8">
         <v>19</v>
@@ -1673,7 +1670,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B9">
         <v>12</v>
@@ -1684,7 +1681,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -1695,7 +1692,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B11">
         <v>8</v>
@@ -1706,7 +1703,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B12">
         <v>19</v>
@@ -1717,7 +1714,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B13">
         <v>10</v>
@@ -1728,7 +1725,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B14">
         <v>5</v>
@@ -1739,7 +1736,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -1750,7 +1747,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B16">
         <v>6</v>
@@ -1761,7 +1758,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -1772,7 +1769,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B18">
         <v>19</v>
@@ -1783,7 +1780,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B19">
         <v>5</v>
@@ -1794,7 +1791,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B20">
         <v>3</v>
@@ -1805,7 +1802,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B21">
         <v>15</v>
@@ -1816,7 +1813,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B22">
         <v>11</v>
@@ -1827,7 +1824,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B23">
         <v>15</v>
@@ -1838,7 +1835,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B24">
         <v>3</v>
@@ -1849,7 +1846,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B25">
         <v>3</v>
@@ -1876,7 +1873,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B1" t="s">
         <v>7</v>
@@ -1884,7 +1881,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B2">
         <v>10</v>
@@ -1892,7 +1889,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B3">
         <v>16</v>
@@ -1900,7 +1897,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B4">
         <v>10</v>
@@ -1908,7 +1905,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B5">
         <v>11</v>
@@ -1916,7 +1913,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B6">
         <v>17</v>
@@ -1924,7 +1921,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B7">
         <v>15</v>
@@ -1932,7 +1929,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B8">
         <v>13</v>
@@ -1940,7 +1937,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B9">
         <v>15</v>
@@ -1948,7 +1945,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B10">
         <v>20</v>
@@ -1956,7 +1953,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B11">
         <v>13</v>
@@ -1964,7 +1961,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B12">
         <v>18</v>
@@ -1972,7 +1969,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B13">
         <v>12</v>
@@ -1980,7 +1977,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B14">
         <v>12</v>
@@ -1988,7 +1985,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B15">
         <v>12</v>
@@ -1996,7 +1993,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B16">
         <v>16</v>
@@ -2004,7 +2001,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B17">
         <v>14</v>
@@ -2012,7 +2009,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B18">
         <v>16</v>
@@ -2020,7 +2017,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B19">
         <v>15</v>
@@ -2028,7 +2025,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B20">
         <v>10</v>
@@ -2036,7 +2033,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B21">
         <v>15</v>
@@ -2044,7 +2041,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B22">
         <v>19</v>
@@ -2052,7 +2049,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B23">
         <v>12</v>
@@ -2060,7 +2057,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B24">
         <v>20</v>
@@ -2068,7 +2065,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B25">
         <v>12</v>
@@ -2083,7 +2080,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3788A93-7501-4F5D-9E8F-38D329CC85EC}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
@@ -2091,16 +2088,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -2108,55 +2105,55 @@
         <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C2" t="s">
         <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -2176,24 +2173,24 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B1" t="s">
         <v>12</v>
       </c>
       <c r="C1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" t="s">
         <v>66</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>67</v>
-      </c>
-      <c r="E1" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B2">
         <v>48</v>
@@ -2210,7 +2207,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B3">
         <v>60</v>
@@ -2227,7 +2224,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B4">
         <v>58</v>
@@ -2244,7 +2241,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B5">
         <v>51</v>
@@ -2261,7 +2258,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B6">
         <v>37</v>
@@ -2278,7 +2275,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B7">
         <v>34</v>
@@ -2295,7 +2292,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B8">
         <v>45</v>
@@ -2312,7 +2309,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B9">
         <v>41</v>
@@ -2329,7 +2326,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B10">
         <v>55</v>
@@ -2346,7 +2343,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B11">
         <v>59</v>
@@ -2363,7 +2360,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B12">
         <v>60</v>
@@ -2380,7 +2377,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B13">
         <v>41</v>
@@ -2397,7 +2394,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B14">
         <v>46</v>
@@ -2414,7 +2411,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B15">
         <v>38</v>
@@ -2431,7 +2428,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B16">
         <v>46</v>
@@ -2448,7 +2445,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B17">
         <v>45</v>
@@ -2465,7 +2462,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B18">
         <v>41</v>
@@ -2482,7 +2479,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B19">
         <v>46</v>
@@ -2499,7 +2496,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B20">
         <v>52</v>
@@ -2516,7 +2513,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B21">
         <v>56</v>
@@ -2533,7 +2530,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B22">
         <v>33</v>
@@ -2550,7 +2547,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B23">
         <v>43</v>
@@ -2567,7 +2564,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B24">
         <v>57</v>
@@ -2584,7 +2581,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B25">
         <v>32</v>

</xml_diff>

<commit_message>
Moved handling of topology to input data import. Fixed error in input data.
</commit_message>
<xml_diff>
--- a/input_data/input_data_V3.xlsx
+++ b/input_data/input_data_V3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dsdennis\HOPE\Predicer\input_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B96AC75-ECF7-40C9-AD56-759F416A340C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F7A6982-F5D8-4031-9594-F9C0309A1C08}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="0" windowWidth="20460" windowHeight="10920" tabRatio="796" activeTab="2" xr2:uid="{788BFBD1-D930-4535-8A91-D85C56924796}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="796" activeTab="2" xr2:uid="{788BFBD1-D930-4535-8A91-D85C56924796}"/>
   </bookViews>
   <sheets>
     <sheet name="nodes" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="49">
   <si>
     <t>node</t>
   </si>
@@ -139,78 +139,6 @@
   </si>
   <si>
     <t>t</t>
-  </si>
-  <si>
-    <t>t1</t>
-  </si>
-  <si>
-    <t>t2</t>
-  </si>
-  <si>
-    <t>t3</t>
-  </si>
-  <si>
-    <t>t4</t>
-  </si>
-  <si>
-    <t>t5</t>
-  </si>
-  <si>
-    <t>t6</t>
-  </si>
-  <si>
-    <t>t7</t>
-  </si>
-  <si>
-    <t>t8</t>
-  </si>
-  <si>
-    <t>t9</t>
-  </si>
-  <si>
-    <t>t10</t>
-  </si>
-  <si>
-    <t>t11</t>
-  </si>
-  <si>
-    <t>t12</t>
-  </si>
-  <si>
-    <t>t13</t>
-  </si>
-  <si>
-    <t>t14</t>
-  </si>
-  <si>
-    <t>t15</t>
-  </si>
-  <si>
-    <t>t16</t>
-  </si>
-  <si>
-    <t>t17</t>
-  </si>
-  <si>
-    <t>t18</t>
-  </si>
-  <si>
-    <t>t19</t>
-  </si>
-  <si>
-    <t>t20</t>
-  </si>
-  <si>
-    <t>t21</t>
-  </si>
-  <si>
-    <t>t22</t>
-  </si>
-  <si>
-    <t>t23</t>
-  </si>
-  <si>
-    <t>t24</t>
   </si>
   <si>
     <t>market</t>
@@ -300,8 +228,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -635,7 +564,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>58</v>
+        <v>34</v>
       </c>
       <c r="E1" t="s">
         <v>6</v>
@@ -771,7 +700,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>60</v>
+        <v>36</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -837,7 +766,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -856,7 +785,7 @@
         <v>15</v>
       </c>
       <c r="D1" t="s">
-        <v>58</v>
+        <v>34</v>
       </c>
       <c r="E1" t="s">
         <v>18</v>
@@ -1007,7 +936,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -1079,7 +1008,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1100,7 +1029,7 @@
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>59</v>
+        <v>35</v>
       </c>
       <c r="E1" t="s">
         <v>16</v>
@@ -1271,7 +1200,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="B10" t="s">
         <v>28</v>
@@ -1291,13 +1220,13 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="B11" t="s">
         <v>30</v>
       </c>
       <c r="C11" t="s">
-        <v>60</v>
+        <v>36</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -1356,15 +1285,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77A4637A-7829-48D6-AE54-2E654AB1A427}">
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>32</v>
       </c>
@@ -1372,197 +1301,221 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>33</v>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>0</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>34</v>
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>4.1666666666666699E-2</v>
       </c>
       <c r="B3">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>35</v>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>8.3333333333333301E-2</v>
       </c>
       <c r="B4">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>36</v>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>0.125</v>
       </c>
       <c r="B5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>37</v>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>0.16666666666666699</v>
       </c>
       <c r="B6">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>38</v>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>0.20833333333333301</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>39</v>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>0.25</v>
       </c>
       <c r="B8">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>40</v>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>0.29166666666666702</v>
       </c>
       <c r="B9">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>41</v>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>0.33333333333333298</v>
       </c>
       <c r="B10">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>42</v>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>0.375</v>
       </c>
       <c r="B11">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>43</v>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>0.41666666666666702</v>
       </c>
       <c r="B12">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>44</v>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>0.45833333333333298</v>
       </c>
       <c r="B13">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>45</v>
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>0.5</v>
       </c>
       <c r="B14">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>46</v>
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>0.54166666666666696</v>
       </c>
       <c r="B15">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>47</v>
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>0.58333333333333304</v>
       </c>
       <c r="B16">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>48</v>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>0.625</v>
       </c>
       <c r="B17">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>49</v>
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>0.66666666666666696</v>
       </c>
       <c r="B18">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>50</v>
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>0.70833333333333304</v>
       </c>
       <c r="B19">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>51</v>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>0.75</v>
       </c>
       <c r="B20">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>52</v>
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>0.79166666666666696</v>
       </c>
       <c r="B21">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>53</v>
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>0.83333333333333304</v>
       </c>
       <c r="B22">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>54</v>
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>0.875</v>
       </c>
       <c r="B23">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>55</v>
+      <c r="E23" s="1"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>0.91666666666666696</v>
       </c>
       <c r="B24">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>56</v>
+      <c r="E24" s="1"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>0.95833333333333304</v>
       </c>
       <c r="B25">
         <v>0.6</v>
       </c>
+      <c r="E25" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1575,7 +1528,7 @@
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2:A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1585,274 +1538,274 @@
         <v>32</v>
       </c>
       <c r="B1" t="s">
-        <v>60</v>
+        <v>36</v>
       </c>
       <c r="C1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>33</v>
+      <c r="A2" s="1">
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>12</v>
+        <v>-12</v>
       </c>
       <c r="C2">
-        <v>3</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>34</v>
+      <c r="A3" s="1">
+        <v>4.1666666666666699E-2</v>
       </c>
       <c r="B3">
-        <v>15</v>
+        <v>-15</v>
       </c>
       <c r="C3">
-        <v>5</v>
+        <v>-5</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>35</v>
+      <c r="A4" s="1">
+        <v>8.3333333333333301E-2</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
       <c r="C4">
-        <v>6</v>
+        <v>-6</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>36</v>
+      <c r="A5" s="1">
+        <v>0.125</v>
       </c>
       <c r="B5">
-        <v>15</v>
+        <v>-15</v>
       </c>
       <c r="C5">
-        <v>3</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>37</v>
+      <c r="A6" s="1">
+        <v>0.16666666666666699</v>
       </c>
       <c r="B6">
-        <v>3</v>
+        <v>-3</v>
       </c>
       <c r="C6">
-        <v>4</v>
+        <v>-4</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>38</v>
+      <c r="A7" s="1">
+        <v>0.20833333333333301</v>
       </c>
       <c r="B7">
-        <v>9</v>
+        <v>-9</v>
       </c>
       <c r="C7">
-        <v>5</v>
+        <v>-5</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>39</v>
+      <c r="A8" s="1">
+        <v>0.25</v>
       </c>
       <c r="B8">
-        <v>19</v>
+        <v>-19</v>
       </c>
       <c r="C8">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>40</v>
+      <c r="A9" s="1">
+        <v>0.29166666666666702</v>
       </c>
       <c r="B9">
-        <v>12</v>
+        <v>-12</v>
       </c>
       <c r="C9">
-        <v>2</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>41</v>
+      <c r="A10" s="1">
+        <v>0.33333333333333298</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="C10">
-        <v>2</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>42</v>
+      <c r="A11" s="1">
+        <v>0.375</v>
       </c>
       <c r="B11">
-        <v>8</v>
+        <v>-8</v>
       </c>
       <c r="C11">
-        <v>5</v>
+        <v>-5</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>43</v>
+      <c r="A12" s="1">
+        <v>0.41666666666666702</v>
       </c>
       <c r="B12">
-        <v>19</v>
+        <v>-19</v>
       </c>
       <c r="C12">
-        <v>2</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>44</v>
+      <c r="A13" s="1">
+        <v>0.45833333333333298</v>
       </c>
       <c r="B13">
-        <v>10</v>
+        <v>-10</v>
       </c>
       <c r="C13">
-        <v>6</v>
+        <v>-6</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>45</v>
+      <c r="A14" s="1">
+        <v>0.5</v>
       </c>
       <c r="B14">
-        <v>5</v>
+        <v>-5</v>
       </c>
       <c r="C14">
-        <v>4</v>
+        <v>-4</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>46</v>
+      <c r="A15" s="1">
+        <v>0.54166666666666696</v>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="C15">
-        <v>3</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>47</v>
+      <c r="A16" s="1">
+        <v>0.58333333333333304</v>
       </c>
       <c r="B16">
-        <v>6</v>
+        <v>-6</v>
       </c>
       <c r="C16">
-        <v>5</v>
+        <v>-5</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>48</v>
+      <c r="A17" s="1">
+        <v>0.625</v>
       </c>
       <c r="B17">
         <v>0</v>
       </c>
       <c r="C17">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>49</v>
+      <c r="A18" s="1">
+        <v>0.66666666666666696</v>
       </c>
       <c r="B18">
-        <v>19</v>
+        <v>-19</v>
       </c>
       <c r="C18">
-        <v>5</v>
+        <v>-5</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>50</v>
+      <c r="A19" s="1">
+        <v>0.70833333333333304</v>
       </c>
       <c r="B19">
-        <v>5</v>
+        <v>-5</v>
       </c>
       <c r="C19">
-        <v>4</v>
+        <v>-4</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>51</v>
+      <c r="A20" s="1">
+        <v>0.75</v>
       </c>
       <c r="B20">
-        <v>3</v>
+        <v>-3</v>
       </c>
       <c r="C20">
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>52</v>
+      <c r="A21" s="1">
+        <v>0.79166666666666696</v>
       </c>
       <c r="B21">
-        <v>15</v>
+        <v>-15</v>
       </c>
       <c r="C21">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>53</v>
+      <c r="A22" s="1">
+        <v>0.83333333333333304</v>
       </c>
       <c r="B22">
-        <v>11</v>
+        <v>-11</v>
       </c>
       <c r="C22">
-        <v>4</v>
+        <v>-4</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>54</v>
+      <c r="A23" s="1">
+        <v>0.875</v>
       </c>
       <c r="B23">
-        <v>15</v>
+        <v>-15</v>
       </c>
       <c r="C23">
-        <v>5</v>
+        <v>-5</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>55</v>
+      <c r="A24" s="1">
+        <v>0.91666666666666696</v>
       </c>
       <c r="B24">
-        <v>3</v>
+        <v>-3</v>
       </c>
       <c r="C24">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>56</v>
+      <c r="A25" s="1">
+        <v>0.95833333333333304</v>
       </c>
       <c r="B25">
-        <v>3</v>
+        <v>-3</v>
       </c>
       <c r="C25">
-        <v>3</v>
+        <v>-3</v>
       </c>
     </row>
   </sheetData>
@@ -1866,7 +1819,7 @@
   <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A2" sqref="A2:A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1880,192 +1833,192 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>33</v>
+      <c r="A2" s="1">
+        <v>0</v>
       </c>
       <c r="B2">
         <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>34</v>
+      <c r="A3" s="1">
+        <v>4.1666666666666699E-2</v>
       </c>
       <c r="B3">
         <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>35</v>
+      <c r="A4" s="1">
+        <v>8.3333333333333301E-2</v>
       </c>
       <c r="B4">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>36</v>
+      <c r="A5" s="1">
+        <v>0.125</v>
       </c>
       <c r="B5">
         <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>37</v>
+      <c r="A6" s="1">
+        <v>0.16666666666666699</v>
       </c>
       <c r="B6">
         <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>38</v>
+      <c r="A7" s="1">
+        <v>0.20833333333333301</v>
       </c>
       <c r="B7">
         <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>39</v>
+      <c r="A8" s="1">
+        <v>0.25</v>
       </c>
       <c r="B8">
         <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>40</v>
+      <c r="A9" s="1">
+        <v>0.29166666666666702</v>
       </c>
       <c r="B9">
         <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>41</v>
+      <c r="A10" s="1">
+        <v>0.33333333333333298</v>
       </c>
       <c r="B10">
         <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>42</v>
+      <c r="A11" s="1">
+        <v>0.375</v>
       </c>
       <c r="B11">
         <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>43</v>
+      <c r="A12" s="1">
+        <v>0.41666666666666702</v>
       </c>
       <c r="B12">
         <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>44</v>
+      <c r="A13" s="1">
+        <v>0.45833333333333298</v>
       </c>
       <c r="B13">
         <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>45</v>
+      <c r="A14" s="1">
+        <v>0.5</v>
       </c>
       <c r="B14">
         <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>46</v>
+      <c r="A15" s="1">
+        <v>0.54166666666666696</v>
       </c>
       <c r="B15">
         <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>47</v>
+      <c r="A16" s="1">
+        <v>0.58333333333333304</v>
       </c>
       <c r="B16">
         <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>48</v>
+      <c r="A17" s="1">
+        <v>0.625</v>
       </c>
       <c r="B17">
         <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>49</v>
+      <c r="A18" s="1">
+        <v>0.66666666666666696</v>
       </c>
       <c r="B18">
         <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>50</v>
+      <c r="A19" s="1">
+        <v>0.70833333333333304</v>
       </c>
       <c r="B19">
         <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>51</v>
+      <c r="A20" s="1">
+        <v>0.75</v>
       </c>
       <c r="B20">
         <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>52</v>
+      <c r="A21" s="1">
+        <v>0.79166666666666696</v>
       </c>
       <c r="B21">
         <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>53</v>
+      <c r="A22" s="1">
+        <v>0.83333333333333304</v>
       </c>
       <c r="B22">
         <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>54</v>
+      <c r="A23" s="1">
+        <v>0.875</v>
       </c>
       <c r="B23">
         <v>12</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>55</v>
+      <c r="A24" s="1">
+        <v>0.91666666666666696</v>
       </c>
       <c r="B24">
         <v>20</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>56</v>
+      <c r="A25" s="1">
+        <v>0.95833333333333304</v>
       </c>
       <c r="B25">
         <v>12</v>
@@ -2088,16 +2041,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>57</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
-        <v>63</v>
+        <v>39</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>68</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -2105,55 +2058,55 @@
         <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>64</v>
+        <v>40</v>
       </c>
       <c r="C2" t="s">
         <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>69</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="B3" t="s">
-        <v>62</v>
+        <v>38</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>70</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>66</v>
+        <v>42</v>
       </c>
       <c r="B4" t="s">
-        <v>62</v>
+        <v>38</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>72</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>67</v>
+        <v>43</v>
       </c>
       <c r="B5" t="s">
-        <v>62</v>
+        <v>38</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>71</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -2165,8 +2118,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF6DDD9A-EF34-4108-8532-230729E9C708}">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2179,18 +2132,18 @@
         <v>12</v>
       </c>
       <c r="C1" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="D1" t="s">
-        <v>66</v>
+        <v>42</v>
       </c>
       <c r="E1" t="s">
-        <v>67</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>33</v>
+      <c r="A2" s="1">
+        <v>0</v>
       </c>
       <c r="B2">
         <v>48</v>
@@ -2206,8 +2159,8 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>34</v>
+      <c r="A3" s="1">
+        <v>4.1666666666666699E-2</v>
       </c>
       <c r="B3">
         <v>60</v>
@@ -2223,8 +2176,8 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>35</v>
+      <c r="A4" s="1">
+        <v>8.3333333333333301E-2</v>
       </c>
       <c r="B4">
         <v>58</v>
@@ -2240,8 +2193,8 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>36</v>
+      <c r="A5" s="1">
+        <v>0.125</v>
       </c>
       <c r="B5">
         <v>51</v>
@@ -2257,8 +2210,8 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>37</v>
+      <c r="A6" s="1">
+        <v>0.16666666666666699</v>
       </c>
       <c r="B6">
         <v>37</v>
@@ -2274,8 +2227,8 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>38</v>
+      <c r="A7" s="1">
+        <v>0.20833333333333301</v>
       </c>
       <c r="B7">
         <v>34</v>
@@ -2291,8 +2244,8 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>39</v>
+      <c r="A8" s="1">
+        <v>0.25</v>
       </c>
       <c r="B8">
         <v>45</v>
@@ -2308,8 +2261,8 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>40</v>
+      <c r="A9" s="1">
+        <v>0.29166666666666702</v>
       </c>
       <c r="B9">
         <v>41</v>
@@ -2325,8 +2278,8 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>41</v>
+      <c r="A10" s="1">
+        <v>0.33333333333333298</v>
       </c>
       <c r="B10">
         <v>55</v>
@@ -2342,8 +2295,8 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>42</v>
+      <c r="A11" s="1">
+        <v>0.375</v>
       </c>
       <c r="B11">
         <v>59</v>
@@ -2359,8 +2312,8 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>43</v>
+      <c r="A12" s="1">
+        <v>0.41666666666666702</v>
       </c>
       <c r="B12">
         <v>60</v>
@@ -2376,8 +2329,8 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>44</v>
+      <c r="A13" s="1">
+        <v>0.45833333333333298</v>
       </c>
       <c r="B13">
         <v>41</v>
@@ -2393,8 +2346,8 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>45</v>
+      <c r="A14" s="1">
+        <v>0.5</v>
       </c>
       <c r="B14">
         <v>46</v>
@@ -2410,8 +2363,8 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>46</v>
+      <c r="A15" s="1">
+        <v>0.54166666666666696</v>
       </c>
       <c r="B15">
         <v>38</v>
@@ -2427,8 +2380,8 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>47</v>
+      <c r="A16" s="1">
+        <v>0.58333333333333304</v>
       </c>
       <c r="B16">
         <v>46</v>
@@ -2444,8 +2397,8 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>48</v>
+      <c r="A17" s="1">
+        <v>0.625</v>
       </c>
       <c r="B17">
         <v>45</v>
@@ -2461,8 +2414,8 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>49</v>
+      <c r="A18" s="1">
+        <v>0.66666666666666696</v>
       </c>
       <c r="B18">
         <v>41</v>
@@ -2478,8 +2431,8 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>50</v>
+      <c r="A19" s="1">
+        <v>0.70833333333333304</v>
       </c>
       <c r="B19">
         <v>46</v>
@@ -2495,8 +2448,8 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>51</v>
+      <c r="A20" s="1">
+        <v>0.75</v>
       </c>
       <c r="B20">
         <v>52</v>
@@ -2512,8 +2465,8 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>52</v>
+      <c r="A21" s="1">
+        <v>0.79166666666666696</v>
       </c>
       <c r="B21">
         <v>56</v>
@@ -2529,8 +2482,8 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>53</v>
+      <c r="A22" s="1">
+        <v>0.83333333333333304</v>
       </c>
       <c r="B22">
         <v>33</v>
@@ -2546,8 +2499,8 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>54</v>
+      <c r="A23" s="1">
+        <v>0.875</v>
       </c>
       <c r="B23">
         <v>43</v>
@@ -2563,8 +2516,8 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>55</v>
+      <c r="A24" s="1">
+        <v>0.91666666666666696</v>
       </c>
       <c r="B24">
         <v>57</v>
@@ -2580,8 +2533,8 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>56</v>
+      <c r="A25" s="1">
+        <v>0.95833333333333304</v>
       </c>
       <c r="B25">
         <v>32</v>

</xml_diff>

<commit_message>
Added reserves to model.
</commit_message>
<xml_diff>
--- a/input_data/input_data_V3.xlsx
+++ b/input_data/input_data_V3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dsdennis\HOPE\Predicer\input_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F7A6982-F5D8-4031-9594-F9C0309A1C08}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA12B93B-BB2E-425C-8F05-0379623D01F0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="796" activeTab="2" xr2:uid="{788BFBD1-D930-4535-8A91-D85C56924796}"/>
+    <workbookView xWindow="-57720" yWindow="-6465" windowWidth="29040" windowHeight="17640" tabRatio="796" activeTab="7" xr2:uid="{788BFBD1-D930-4535-8A91-D85C56924796}"/>
   </bookViews>
   <sheets>
     <sheet name="nodes" sheetId="1" r:id="rId1"/>
@@ -228,9 +228,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -766,7 +767,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -832,10 +833,10 @@
         <v>1</v>
       </c>
       <c r="I2">
-        <v>0.2</v>
+        <v>0.8</v>
       </c>
       <c r="J2">
-        <v>0.2</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -864,10 +865,10 @@
         <v>1</v>
       </c>
       <c r="I3">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="J3">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -896,10 +897,10 @@
         <v>1</v>
       </c>
       <c r="I4">
-        <v>0.3</v>
+        <v>0.8</v>
       </c>
       <c r="J4">
-        <v>0.3</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -1007,7 +1008,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A86A8A7-FD76-4891-A53C-CBB095359118}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
@@ -1525,15 +1526,18 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F87DD44-A1AD-4241-AED7-C48CC9DEE2E2}">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A25"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="7" max="7" width="9.140625" style="2"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>32</v>
       </c>
@@ -1544,166 +1548,168 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>-12</v>
+        <v>-4</v>
       </c>
       <c r="C2">
         <v>-3</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F2" s="1"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>4.1666666666666699E-2</v>
       </c>
       <c r="B3">
-        <v>-15</v>
+        <v>-5</v>
       </c>
       <c r="C3">
         <v>-5</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>8.3333333333333301E-2</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>-4</v>
       </c>
       <c r="C4">
         <v>-6</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>0.125</v>
       </c>
       <c r="B5">
-        <v>-15</v>
+        <v>-2</v>
       </c>
       <c r="C5">
         <v>-3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>0.16666666666666699</v>
       </c>
       <c r="B6">
-        <v>-3</v>
+        <v>-7</v>
       </c>
       <c r="C6">
         <v>-4</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>0.20833333333333301</v>
       </c>
       <c r="B7">
-        <v>-9</v>
+        <v>-5</v>
       </c>
       <c r="C7">
         <v>-5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>0.25</v>
       </c>
       <c r="B8">
-        <v>-19</v>
+        <v>-14</v>
       </c>
       <c r="C8">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>0.29166666666666702</v>
       </c>
       <c r="B9">
-        <v>-12</v>
+        <v>-20</v>
       </c>
       <c r="C9">
         <v>-2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>0.33333333333333298</v>
       </c>
       <c r="B10">
-        <v>-1</v>
+        <v>-13</v>
       </c>
       <c r="C10">
         <v>-2</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>0.375</v>
       </c>
       <c r="B11">
-        <v>-8</v>
+        <v>-12</v>
       </c>
       <c r="C11">
         <v>-5</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>0.41666666666666702</v>
       </c>
       <c r="B12">
-        <v>-19</v>
+        <v>-13</v>
       </c>
       <c r="C12">
         <v>-2</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>0.45833333333333298</v>
       </c>
       <c r="B13">
-        <v>-10</v>
+        <v>-14</v>
       </c>
       <c r="C13">
         <v>-6</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>0.5</v>
       </c>
       <c r="B14">
-        <v>-5</v>
+        <v>-18</v>
       </c>
       <c r="C14">
         <v>-4</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>0.54166666666666696</v>
       </c>
       <c r="B15">
-        <v>-1</v>
+        <v>-14</v>
       </c>
       <c r="C15">
         <v>-3</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>0.58333333333333304</v>
       </c>
       <c r="B16">
-        <v>-6</v>
+        <v>-15</v>
       </c>
       <c r="C16">
         <v>-5</v>
@@ -1714,7 +1720,7 @@
         <v>0.625</v>
       </c>
       <c r="B17">
-        <v>0</v>
+        <v>-14</v>
       </c>
       <c r="C17">
         <v>-1</v>
@@ -1725,7 +1731,7 @@
         <v>0.66666666666666696</v>
       </c>
       <c r="B18">
-        <v>-19</v>
+        <v>-20</v>
       </c>
       <c r="C18">
         <v>-5</v>
@@ -1736,7 +1742,7 @@
         <v>0.70833333333333304</v>
       </c>
       <c r="B19">
-        <v>-5</v>
+        <v>-20</v>
       </c>
       <c r="C19">
         <v>-4</v>
@@ -1747,7 +1753,7 @@
         <v>0.75</v>
       </c>
       <c r="B20">
-        <v>-3</v>
+        <v>-20</v>
       </c>
       <c r="C20">
         <v>0</v>
@@ -1758,7 +1764,7 @@
         <v>0.79166666666666696</v>
       </c>
       <c r="B21">
-        <v>-15</v>
+        <v>-20</v>
       </c>
       <c r="C21">
         <v>-1</v>
@@ -1769,7 +1775,7 @@
         <v>0.83333333333333304</v>
       </c>
       <c r="B22">
-        <v>-11</v>
+        <v>-16</v>
       </c>
       <c r="C22">
         <v>-4</v>
@@ -1780,7 +1786,7 @@
         <v>0.875</v>
       </c>
       <c r="B23">
-        <v>-15</v>
+        <v>-14</v>
       </c>
       <c r="C23">
         <v>-5</v>
@@ -1791,7 +1797,7 @@
         <v>0.91666666666666696</v>
       </c>
       <c r="B24">
-        <v>-3</v>
+        <v>-11</v>
       </c>
       <c r="C24">
         <v>-1</v>
@@ -1802,7 +1808,7 @@
         <v>0.95833333333333304</v>
       </c>
       <c r="B25">
-        <v>-3</v>
+        <v>-9</v>
       </c>
       <c r="C25">
         <v>-3</v>
@@ -1811,6 +1817,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1819,7 +1826,7 @@
   <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A25"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1837,7 +1844,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1845,7 +1852,7 @@
         <v>4.1666666666666699E-2</v>
       </c>
       <c r="B3">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1869,7 +1876,7 @@
         <v>0.16666666666666699</v>
       </c>
       <c r="B6">
-        <v>17</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1877,7 +1884,7 @@
         <v>0.20833333333333301</v>
       </c>
       <c r="B7">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1885,7 +1892,7 @@
         <v>0.25</v>
       </c>
       <c r="B8">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -1893,7 +1900,7 @@
         <v>0.29166666666666702</v>
       </c>
       <c r="B9">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -1901,7 +1908,7 @@
         <v>0.33333333333333298</v>
       </c>
       <c r="B10">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -1909,7 +1916,7 @@
         <v>0.375</v>
       </c>
       <c r="B11">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -1917,7 +1924,7 @@
         <v>0.41666666666666702</v>
       </c>
       <c r="B12">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -1925,7 +1932,7 @@
         <v>0.45833333333333298</v>
       </c>
       <c r="B13">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -1933,7 +1940,7 @@
         <v>0.5</v>
       </c>
       <c r="B14">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -1941,7 +1948,7 @@
         <v>0.54166666666666696</v>
       </c>
       <c r="B15">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -1949,7 +1956,7 @@
         <v>0.58333333333333304</v>
       </c>
       <c r="B16">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -1957,7 +1964,7 @@
         <v>0.625</v>
       </c>
       <c r="B17">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -1965,7 +1972,7 @@
         <v>0.66666666666666696</v>
       </c>
       <c r="B18">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -1973,7 +1980,7 @@
         <v>0.70833333333333304</v>
       </c>
       <c r="B19">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -1981,7 +1988,7 @@
         <v>0.75</v>
       </c>
       <c r="B20">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -1989,7 +1996,7 @@
         <v>0.79166666666666696</v>
       </c>
       <c r="B21">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -1997,7 +2004,7 @@
         <v>0.83333333333333304</v>
       </c>
       <c r="B22">
-        <v>19</v>
+        <v>11</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -2005,7 +2012,7 @@
         <v>0.875</v>
       </c>
       <c r="B23">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -2013,7 +2020,7 @@
         <v>0.91666666666666696</v>
       </c>
       <c r="B24">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -2021,7 +2028,7 @@
         <v>0.95833333333333304</v>
       </c>
       <c r="B25">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -2118,9 +2125,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF6DDD9A-EF34-4108-8532-230729E9C708}">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>